<commit_message>
Menambah tabel Daily Scrum
</commit_message>
<xml_diff>
--- a/Meme Agile.xlsx
+++ b/Meme Agile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\Git Collab\kelompok_meme_laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E824C-C264-41A2-81D6-12A5E95B5726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F6AA95-066E-4710-B9A5-7BB816AA24AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD1CD595-25D7-451D-99CB-E4C06CA26580}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,64 +680,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -748,20 +691,71 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,13 +779,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>781049</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>149</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>27773</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -835,13 +829,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>153</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>116122</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -885,13 +879,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>428626</xdr:colOff>
-      <xdr:row>196</xdr:row>
+      <xdr:row>199</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>266701</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>213</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -935,13 +929,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>668162</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>194</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>49184</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -985,13 +979,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>147600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>194</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>43391</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1035,13 +1029,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>752476</xdr:colOff>
-      <xdr:row>196</xdr:row>
+      <xdr:row>199</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>211</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1381,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C4E763-3BF0-4DCE-A690-0A0674D041AB}">
-  <dimension ref="A1:G222"/>
+  <dimension ref="A1:G225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,23 +1393,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="3:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="4" spans="3:5" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="6" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
@@ -1446,18 +1440,18 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D22" s="9" t="s">
@@ -1465,38 +1459,38 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
+      <c r="A25" s="11"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="11" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
+      <c r="A28" s="11"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="11" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="11" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="11"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1504,12 +1498,12 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="11" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="A34" s="11"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1517,17 +1511,17 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="11" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="11" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
+      <c r="A38" s="11"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1535,349 +1529,349 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="11" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
+      <c r="A41" s="11"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="30"/>
+      <c r="A42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F44" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="34" t="s">
+      <c r="G44" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="35">
+      <c r="A45" s="1">
         <v>551</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="36">
+      <c r="G45" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="35">
+      <c r="A46" s="1">
         <v>552</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="D46" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="36" t="s">
+      <c r="E46" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="36">
+      <c r="G46" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="35">
+      <c r="A47" s="1">
         <v>553</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="36" t="s">
+      <c r="D47" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="36" t="s">
+      <c r="E47" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="36" t="s">
+      <c r="F47" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="36">
+      <c r="G47" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="35">
+      <c r="A48" s="1">
         <v>554</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D48" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="36" t="s">
+      <c r="E48" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="36" t="s">
+      <c r="F48" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G48" s="36">
+      <c r="G48" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="35">
+      <c r="A49" s="1">
         <v>555</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="36" t="s">
+      <c r="D49" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="36" t="s">
+      <c r="E49" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F49" s="36" t="s">
+      <c r="F49" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="36">
+      <c r="G49" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="35">
+      <c r="A50" s="1">
         <v>556</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="36" t="s">
+      <c r="D50" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="36" t="s">
+      <c r="F50" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G50" s="36">
+      <c r="G50" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="35">
+      <c r="A51" s="1">
         <v>557</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="36" t="s">
+      <c r="E51" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F51" s="36" t="s">
+      <c r="F51" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="36">
+      <c r="G51" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="35">
+      <c r="A52" s="1">
         <v>558</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="36" t="s">
+      <c r="E52" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F52" s="36" t="s">
+      <c r="F52" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="36">
+      <c r="G52" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="28"/>
     </row>
     <row r="60" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="11"/>
+      <c r="B60" s="28"/>
     </row>
     <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B61" s="12"/>
+      <c r="B61" s="35"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="14"/>
+      <c r="B62" s="26"/>
     </row>
     <row r="63" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="11"/>
+      <c r="B63" s="28"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
+      <c r="A64" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="31">
+      <c r="A65" s="12">
         <v>551</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B65" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="31">
+      <c r="A66" s="12">
         <v>552</v>
       </c>
-      <c r="B66" s="32" t="s">
+      <c r="B66" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A67" s="31">
+      <c r="A67" s="12">
         <v>553</v>
       </c>
-      <c r="B67" s="32" t="s">
+      <c r="B67" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="31">
+      <c r="A68" s="12">
         <v>554</v>
       </c>
-      <c r="B68" s="32" t="s">
+      <c r="B68" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="31">
+      <c r="A69" s="12">
         <v>555</v>
       </c>
-      <c r="B69" s="32" t="s">
+      <c r="B69" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="31">
+      <c r="A70" s="12">
         <v>557</v>
       </c>
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="11"/>
+      <c r="B72" s="28"/>
     </row>
     <row r="73" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="11"/>
+      <c r="B73" s="28"/>
     </row>
     <row r="74" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B74" s="19"/>
+      <c r="B74" s="24"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B75" s="14"/>
+      <c r="B75" s="26"/>
     </row>
     <row r="76" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="18" t="s">
+      <c r="A76" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="18"/>
+      <c r="B76" s="27"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
@@ -1896,34 +1890,34 @@
       </c>
     </row>
     <row r="80" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="11"/>
+      <c r="B80" s="28"/>
     </row>
     <row r="81" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="11"/>
+      <c r="B81" s="28"/>
     </row>
     <row r="82" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B82" s="19"/>
+      <c r="B82" s="24"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B83" s="14"/>
+      <c r="B83" s="26"/>
     </row>
     <row r="84" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="18" t="s">
+      <c r="A84" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B84" s="18"/>
+      <c r="B84" s="27"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
@@ -1942,10 +1936,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D88" s="11"/>
+      <c r="D88" s="28"/>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -1977,7 +1971,7 @@
       <c r="C90" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D90" s="24">
+      <c r="D90" s="10">
         <v>45039</v>
       </c>
       <c r="E90" s="1" t="s">
@@ -1997,7 +1991,7 @@
       <c r="C91" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D91" s="24">
+      <c r="D91" s="10">
         <v>45039</v>
       </c>
       <c r="E91" s="1" t="s">
@@ -2017,7 +2011,7 @@
       <c r="C92" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D92" s="24">
+      <c r="D92" s="10">
         <v>45041</v>
       </c>
       <c r="E92" s="1" t="s">
@@ -2037,7 +2031,7 @@
       <c r="C93" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D93" s="24">
+      <c r="D93" s="10">
         <v>45045</v>
       </c>
       <c r="E93" s="1" t="s">
@@ -2057,7 +2051,7 @@
       <c r="C94" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D94" s="24">
+      <c r="D94" s="10">
         <v>45048</v>
       </c>
       <c r="E94" s="1" t="s">
@@ -2067,370 +2061,410 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C96" s="11" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>6</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>7</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>8</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+    </row>
+    <row r="99" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C99" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D96" s="11"/>
-    </row>
-    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A97" s="27" t="s">
+      <c r="D99" s="28"/>
+    </row>
+    <row r="100" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-    </row>
-    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="B100" s="36"/>
+      <c r="C100" s="36"/>
+    </row>
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-    </row>
-    <row r="102" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-    </row>
-    <row r="103" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
     </row>
-    <row r="106" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="26" t="s">
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+    </row>
+    <row r="109" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-    </row>
-    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="25" t="s">
+      <c r="B109" s="37"/>
+      <c r="C109" s="37"/>
+    </row>
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C110" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="26" t="s">
+    <row r="113" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-    </row>
-    <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="25" t="s">
+      <c r="B113" s="37"/>
+      <c r="C113" s="37"/>
+    </row>
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+    <row r="115" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C115" s="11" t="s">
+    <row r="118" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C118" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D115" s="11"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="29" t="s">
+      <c r="D118" s="28"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B116" s="29"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="29"/>
-      <c r="E116" s="29"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="28" t="s">
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B117" s="28"/>
-      <c r="C117" s="28" t="s">
+      <c r="B120" s="20"/>
+      <c r="C120" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D117" s="28"/>
-      <c r="E117" s="28"/>
-    </row>
-    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="D120" s="20"/>
+      <c r="E120" s="20"/>
+    </row>
+    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+    <row r="122" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E122" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="29" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B121" s="29"/>
-      <c r="C121" s="29"/>
-      <c r="D121" s="29"/>
-      <c r="E121" s="29"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="28" t="s">
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B122" s="28"/>
-      <c r="C122" s="28" t="s">
+      <c r="B125" s="20"/>
+      <c r="C125" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D122" s="28"/>
-      <c r="E122" s="28"/>
-    </row>
-    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="D125" s="20"/>
+      <c r="E125" s="20"/>
+    </row>
+    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C126" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="E126" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E124" s="1" t="s">
+      <c r="E127" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="29" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B126" s="29"/>
-      <c r="C126" s="29"/>
-      <c r="D126" s="29"/>
-      <c r="E126" s="29"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="28" t="s">
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B127" s="28"/>
-      <c r="C127" s="28" t="s">
+      <c r="B130" s="20"/>
+      <c r="C130" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D127" s="28"/>
-      <c r="E127" s="28"/>
-    </row>
-    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+    </row>
+    <row r="131" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+    <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E129" s="1" t="s">
+      <c r="E132" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C131" s="11" t="s">
+    <row r="134" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C134" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D131" s="11"/>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="39" t="s">
+      <c r="D134" s="28"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="174" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C174" s="11" t="s">
+    <row r="177" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C177" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D174" s="11"/>
-    </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="39" t="s">
+      <c r="D177" s="28"/>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="178" spans="3:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C178" s="11" t="s">
+    <row r="181" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C181" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D178" s="11"/>
-    </row>
-    <row r="214" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C214" s="38" t="s">
+      <c r="D181" s="28"/>
+    </row>
+    <row r="217" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C217" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D214" s="38"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="D217" s="21"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F221" t="s">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F224" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F222" t="s">
+    <row r="225" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F225" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A126:E126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="C214:D214"/>
-    <mergeCell ref="A121:E121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="A116:E116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C181:D181"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C177:D177"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A109:C109"/>
+    <mergeCell ref="A113:C113"/>
+    <mergeCell ref="A119:E119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="C120:E120"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A82:B82"/>
     <mergeCell ref="A83:B83"/>
@@ -2444,23 +2478,13 @@
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C178:D178"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A106:C106"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="A129:E129"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C217:D217"/>
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="C125:E125"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Daily Scrum Meeting Report
</commit_message>
<xml_diff>
--- a/Meme Agile.xlsx
+++ b/Meme Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\Git Collab\kelompok_meme_laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEA6490-78E2-4BC2-A144-B3840A0576EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C4CA20-D5F2-4219-AB02-4BD296AB56AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BD1CD595-25D7-451D-99CB-E4C06CA26580}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="163">
   <si>
     <t>Product Backlog &amp; User Story</t>
   </si>
@@ -484,6 +484,36 @@
   </si>
   <si>
     <t>Terlalu banyak item untuk dipilih</t>
+  </si>
+  <si>
+    <t>Mengupgrade UI</t>
+  </si>
+  <si>
+    <t>Design yang pas sangat sulit ditemukan</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Belum di optimisasi</t>
+  </si>
+  <si>
+    <t>Membuat Laporan Trello dan PDF</t>
+  </si>
+  <si>
+    <t>Mengumpulkan semua diskusi menjadi 1</t>
+  </si>
+  <si>
+    <t>Mengupgrade Navigation Bar</t>
+  </si>
+  <si>
+    <t>Menambah Card</t>
+  </si>
+  <si>
+    <t>Bug Visual</t>
+  </si>
+  <si>
+    <t>Tidak bisa di Click</t>
   </si>
 </sst>
 </file>
@@ -738,9 +768,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,60 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,13 +866,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>781049</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1266825</xdr:colOff>
-      <xdr:row>173</xdr:row>
+      <xdr:row>176</xdr:row>
       <xdr:rowOff>27773</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -886,13 +916,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1371600</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>196</xdr:row>
       <xdr:rowOff>116122</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -936,13 +966,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>428626</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>223</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>266701</xdr:colOff>
-      <xdr:row>234</xdr:row>
+      <xdr:row>237</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -986,13 +1016,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>668162</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>218</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>49184</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1036,13 +1066,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>147600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>218</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>43391</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1086,13 +1116,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>752476</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>223</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>235</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1432,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C4E763-3BF0-4DCE-A690-0A0674D041AB}">
-  <dimension ref="A1:G246"/>
+  <dimension ref="A1:G249"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,23 +1480,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="36"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="3:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="4" spans="3:5" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="6" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
@@ -1497,18 +1527,18 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D22" s="9" t="s">
@@ -1597,15 +1627,15 @@
       <c r="A42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="41"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -1815,34 +1845,34 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B59" s="20"/>
+      <c r="B59" s="24"/>
     </row>
     <row r="60" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="20"/>
+      <c r="B60" s="24"/>
     </row>
     <row r="61" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B61" s="43"/>
+      <c r="B61" s="34"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="31"/>
+      <c r="B62" s="29"/>
     </row>
     <row r="63" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="20"/>
+      <c r="B63" s="24"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
@@ -1901,34 +1931,34 @@
       </c>
     </row>
     <row r="72" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="20" t="s">
+      <c r="A72" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="20"/>
+      <c r="B72" s="24"/>
     </row>
     <row r="73" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="20"/>
+      <c r="B73" s="24"/>
     </row>
     <row r="74" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="38" t="s">
+      <c r="A74" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B74" s="38"/>
+      <c r="B74" s="27"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B75" s="31"/>
+      <c r="B75" s="29"/>
     </row>
     <row r="76" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="40" t="s">
+      <c r="A76" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B76" s="40"/>
+      <c r="B76" s="30"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
@@ -1947,34 +1977,34 @@
       </c>
     </row>
     <row r="80" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="20" t="s">
+      <c r="A80" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="20"/>
+      <c r="B80" s="24"/>
     </row>
     <row r="81" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="20" t="s">
+      <c r="A81" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="20"/>
+      <c r="B81" s="24"/>
     </row>
     <row r="82" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="38" t="s">
+      <c r="A82" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B82" s="38"/>
+      <c r="B82" s="27"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="39" t="s">
+      <c r="A83" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B83" s="31"/>
+      <c r="B83" s="29"/>
     </row>
     <row r="84" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="40" t="s">
+      <c r="A84" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B84" s="40"/>
+      <c r="B84" s="30"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
@@ -1993,10 +2023,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C88" s="20" t="s">
+      <c r="C88" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D88" s="20"/>
+      <c r="D88" s="24"/>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -2129,7 +2159,7 @@
         <v>151</v>
       </c>
       <c r="D95" s="10">
-        <v>45107</v>
+        <v>45079</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>152</v>
@@ -2138,578 +2168,680 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>7</v>
       </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
+      <c r="B96" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D96" s="10">
+        <v>45088</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F96" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>8</v>
       </c>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="99" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C99" s="20" t="s">
+      <c r="B97" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D97" s="10">
+        <v>45095</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F97" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>9</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D98" s="10">
+        <v>45098</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F98" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>10</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D99" s="10">
+        <v>45102</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F99" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>11</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D100" s="10">
+        <v>45112</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F100" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C102" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D99" s="20"/>
-    </row>
-    <row r="100" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A100" s="32" t="s">
+      <c r="D102" s="24"/>
+    </row>
+    <row r="103" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B100" s="32"/>
-      <c r="C100" s="32"/>
-    </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+    </row>
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C104" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C103" s="1"/>
-    </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B106" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
     </row>
-    <row r="109" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="33" t="s">
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+    </row>
+    <row r="112" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B109" s="33"/>
-      <c r="C109" s="33"/>
-    </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="B112" s="23"/>
+      <c r="C112" s="23"/>
+    </row>
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="114" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="33" t="s">
+    <row r="116" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B113" s="33"/>
-      <c r="C113" s="33"/>
-    </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="B116" s="23"/>
+      <c r="C116" s="23"/>
+    </row>
+    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+    <row r="118" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1" t="s">
+    <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1" t="s">
+    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="19"/>
-      <c r="B118" s="19"/>
-      <c r="C118" s="19"/>
-    </row>
-    <row r="119" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="33" t="s">
+    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="19"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+    </row>
+    <row r="122" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="B119" s="33"/>
-      <c r="C119" s="33"/>
-    </row>
-    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="B122" s="23"/>
+      <c r="C122" s="23"/>
+    </row>
+    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C124" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C124" s="20" t="s">
+    <row r="127" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C127" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D124" s="20"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="34" t="s">
+      <c r="D127" s="24"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B125" s="34"/>
-      <c r="C125" s="34"/>
-      <c r="D125" s="34"/>
-      <c r="E125" s="34"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="35" t="s">
+      <c r="B128" s="21"/>
+      <c r="C128" s="21"/>
+      <c r="D128" s="21"/>
+      <c r="E128" s="21"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B126" s="35"/>
-      <c r="C126" s="35" t="s">
+      <c r="B129" s="22"/>
+      <c r="C129" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D126" s="35"/>
-      <c r="E126" s="35"/>
-    </row>
-    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="D129" s="22"/>
+      <c r="E129" s="22"/>
+    </row>
+    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E127" s="1" t="s">
+      <c r="E130" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+    <row r="131" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="E131" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="34" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B130" s="34"/>
-      <c r="C130" s="34"/>
-      <c r="D130" s="34"/>
-      <c r="E130" s="34"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="35" t="s">
+      <c r="B133" s="21"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B131" s="35"/>
-      <c r="C131" s="35" t="s">
+      <c r="B134" s="22"/>
+      <c r="C134" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D131" s="35"/>
-      <c r="E131" s="35"/>
-    </row>
-    <row r="132" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="D134" s="22"/>
+      <c r="E134" s="22"/>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B135" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C135" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B136" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E133" s="1" t="s">
+      <c r="E136" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="27" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B135" s="28"/>
-      <c r="C135" s="28"/>
-      <c r="D135" s="28"/>
-      <c r="E135" s="29"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="24" t="s">
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="37"/>
+      <c r="E138" s="38"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B136" s="25"/>
-      <c r="C136" s="24" t="s">
+      <c r="B139" s="43"/>
+      <c r="C139" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D136" s="26"/>
-      <c r="E136" s="25"/>
-    </row>
-    <row r="137" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="D139" s="44"/>
+      <c r="E139" s="43"/>
+    </row>
+    <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B140" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E137" s="1" t="s">
+      <c r="E140" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+    <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B141" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="C141" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D138" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E138" s="1" t="s">
+      <c r="E141" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="27" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="B140" s="28"/>
-      <c r="C140" s="28"/>
-      <c r="D140" s="28"/>
-      <c r="E140" s="29"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="24" t="s">
+      <c r="B143" s="37"/>
+      <c r="C143" s="37"/>
+      <c r="D143" s="37"/>
+      <c r="E143" s="38"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B141" s="25"/>
-      <c r="C141" s="24" t="s">
+      <c r="B144" s="43"/>
+      <c r="C144" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D141" s="26"/>
-      <c r="E141" s="25"/>
-    </row>
-    <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="D144" s="44"/>
+      <c r="E144" s="43"/>
+    </row>
+    <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B145" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C145" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D142" s="1" t="s">
+      <c r="D145" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E142" s="1" t="s">
+      <c r="E145" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D143" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E143" s="1" t="s">
+      <c r="E146" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="27" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B145" s="28"/>
-      <c r="C145" s="28"/>
-      <c r="D145" s="28"/>
-      <c r="E145" s="29"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="24" t="s">
+      <c r="B148" s="37"/>
+      <c r="C148" s="37"/>
+      <c r="D148" s="37"/>
+      <c r="E148" s="38"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B146" s="25"/>
-      <c r="C146" s="24" t="s">
+      <c r="B149" s="43"/>
+      <c r="C149" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D146" s="26"/>
-      <c r="E146" s="25"/>
-    </row>
-    <row r="147" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+      <c r="D149" s="44"/>
+      <c r="E149" s="43"/>
+    </row>
+    <row r="150" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B150" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C150" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E147" s="1" t="s">
+      <c r="E150" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="27" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="B150" s="28"/>
-      <c r="C150" s="28"/>
-      <c r="D150" s="28"/>
-      <c r="E150" s="29"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="24" t="s">
+      <c r="B153" s="37"/>
+      <c r="C153" s="37"/>
+      <c r="D153" s="37"/>
+      <c r="E153" s="38"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B151" s="25"/>
-      <c r="C151" s="24" t="s">
+      <c r="B154" s="43"/>
+      <c r="C154" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D151" s="26"/>
-      <c r="E151" s="25"/>
-    </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+      <c r="D154" s="44"/>
+      <c r="E154" s="43"/>
+    </row>
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B155" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C155" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D152" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="E155" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
-    </row>
-    <row r="155" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C155" s="20" t="s">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+    </row>
+    <row r="158" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C158" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D155" s="20"/>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="18" t="s">
+      <c r="D158" s="24"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="198" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C198" s="20" t="s">
+    <row r="201" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C201" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D198" s="20"/>
-    </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="18" t="s">
+      <c r="D201" s="24"/>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B203" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="202" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C202" s="20" t="s">
+    <row r="205" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C205" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D202" s="20"/>
-    </row>
-    <row r="238" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C238" s="44" t="s">
+      <c r="D205" s="24"/>
+    </row>
+    <row r="241" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C241" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D238" s="44"/>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
+      <c r="D241" s="20"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F245" t="s">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F248" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F246" t="s">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F249" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="C238:D238"/>
-    <mergeCell ref="A130:E130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="A113:C113"/>
-    <mergeCell ref="C202:D202"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="C154:E154"/>
+    <mergeCell ref="A148:E148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="C149:E149"/>
+    <mergeCell ref="A143:E143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="C144:E144"/>
+    <mergeCell ref="A138:E138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C201:D201"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="A103:C103"/>
+    <mergeCell ref="A112:C112"/>
+    <mergeCell ref="A122:C122"/>
+    <mergeCell ref="A128:E128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="A153:E153"/>
+    <mergeCell ref="C127:D127"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="A82:B82"/>
     <mergeCell ref="A83:B83"/>
@@ -2726,34 +2858,12 @@
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C198:D198"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A109:C109"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A125:E125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="C126:E126"/>
-    <mergeCell ref="A150:E150"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="C151:E151"/>
-    <mergeCell ref="A145:E145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="A140:E140"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="C141:E141"/>
-    <mergeCell ref="A135:E135"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C241:D241"/>
+    <mergeCell ref="A133:E133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="A116:C116"/>
+    <mergeCell ref="C205:D205"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Meme excel lagi
</commit_message>
<xml_diff>
--- a/Meme Agile.xlsx
+++ b/Meme Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\github\kelompok_meme_laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C73BD9-75AF-405F-A30F-219EB860ECF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4B62FC-9F1F-482D-9D2D-040F2A732E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BD1CD595-25D7-451D-99CB-E4C06CA26580}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="173">
   <si>
     <t>Product Backlog &amp; User Story</t>
   </si>
@@ -538,6 +538,12 @@
   </si>
   <si>
     <t>Membantu Customer proses pesan aplikasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> agar tidak salah menekan dan membuang waktu saat membeli</t>
+  </si>
+  <si>
+    <t>Ingin Navigation Bar lebih mudah liat</t>
   </si>
 </sst>
 </file>
@@ -792,8 +798,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -801,51 +855,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -855,16 +870,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1488,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C4E763-3BF0-4DCE-A690-0A0674D041AB}">
   <dimension ref="A1:G279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1504,23 +1510,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" s="4" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="3:5" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="4" spans="3:5" s="5" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="6" spans="3:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D6" s="6" t="s">
@@ -1551,18 +1557,18 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="20" spans="1:5" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="D22" s="9" t="s">
@@ -1651,15 +1657,15 @@
       <c r="A42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="44"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="27"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
@@ -1891,16 +1897,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>560</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
+      <c r="B54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" s="16">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
@@ -1914,34 +1932,34 @@
       <c r="G55" s="16"/>
     </row>
     <row r="62" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="24"/>
+      <c r="B62" s="21"/>
     </row>
     <row r="63" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B63" s="24"/>
+      <c r="B63" s="21"/>
     </row>
     <row r="64" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="40"/>
+      <c r="B64" s="43"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="35"/>
+      <c r="B65" s="24"/>
     </row>
     <row r="66" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B66" s="24"/>
+      <c r="B66" s="21"/>
     </row>
     <row r="67" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="14" t="s">
@@ -2000,34 +2018,34 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A75" s="24" t="s">
+      <c r="A75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B75" s="24"/>
+      <c r="B75" s="21"/>
     </row>
     <row r="76" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A76" s="24" t="s">
+      <c r="A76" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="24"/>
+      <c r="B76" s="21"/>
     </row>
     <row r="77" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A77" s="33" t="s">
+      <c r="A77" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B77" s="33"/>
+      <c r="B77" s="22"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B78" s="35"/>
+      <c r="B78" s="24"/>
     </row>
     <row r="79" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A79" s="36" t="s">
+      <c r="A79" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B79" s="36"/>
+      <c r="B79" s="20"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
@@ -2046,34 +2064,34 @@
       </c>
     </row>
     <row r="83" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A83" s="24" t="s">
+      <c r="A83" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="24"/>
+      <c r="B83" s="21"/>
     </row>
     <row r="84" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A84" s="24" t="s">
+      <c r="A84" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B84" s="24"/>
+      <c r="B84" s="21"/>
     </row>
     <row r="85" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A85" s="33" t="s">
+      <c r="A85" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="33"/>
+      <c r="B85" s="22"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="34" t="s">
+      <c r="A86" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B86" s="35"/>
+      <c r="B86" s="24"/>
     </row>
     <row r="87" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A87" s="36" t="s">
+      <c r="A87" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="36"/>
+      <c r="B87" s="20"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
@@ -2092,32 +2110,32 @@
       </c>
     </row>
     <row r="91" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A91" s="24" t="s">
+      <c r="A91" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="24"/>
+      <c r="B91" s="21"/>
     </row>
     <row r="92" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A92" s="24" t="s">
+      <c r="A92" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="B92" s="24"/>
+      <c r="B92" s="21"/>
     </row>
     <row r="93" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A93" s="33" t="s">
+      <c r="A93" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B93" s="33"/>
+      <c r="B93" s="22"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="34"/>
-      <c r="B94" s="35"/>
+      <c r="A94" s="23"/>
+      <c r="B94" s="24"/>
     </row>
     <row r="95" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A95" s="36" t="s">
+      <c r="A95" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B95" s="36"/>
+      <c r="B95" s="20"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
@@ -2144,32 +2162,32 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A100" s="24" t="s">
+      <c r="A100" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="24"/>
+      <c r="B100" s="21"/>
     </row>
     <row r="101" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A101" s="24" t="s">
+      <c r="A101" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="B101" s="24"/>
+      <c r="B101" s="21"/>
     </row>
     <row r="102" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A102" s="33" t="s">
+      <c r="A102" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B102" s="33"/>
+      <c r="B102" s="22"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A103" s="34"/>
-      <c r="B103" s="35"/>
+      <c r="A103" s="23"/>
+      <c r="B103" s="24"/>
     </row>
     <row r="104" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A104" s="36" t="s">
+      <c r="A104" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B104" s="36"/>
+      <c r="B104" s="20"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
@@ -2186,10 +2204,10 @@
       <c r="B106" s="1"/>
     </row>
     <row r="108" spans="1:6" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C108" s="24" t="s">
+      <c r="C108" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D108" s="24"/>
+      <c r="D108" s="21"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
@@ -2432,17 +2450,17 @@
       </c>
     </row>
     <row r="122" spans="1:6" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C122" s="24" t="s">
+      <c r="C122" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D122" s="24"/>
+      <c r="D122" s="21"/>
     </row>
     <row r="123" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A123" s="41" t="s">
+      <c r="A123" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B123" s="41"/>
-      <c r="C123" s="41"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="35"/>
     </row>
     <row r="124" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
@@ -2504,11 +2522,11 @@
       <c r="C130" s="1"/>
     </row>
     <row r="132" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A132" s="23" t="s">
+      <c r="A132" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B132" s="23"/>
-      <c r="C132" s="23"/>
+      <c r="B132" s="36"/>
+      <c r="C132" s="36"/>
     </row>
     <row r="133" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
@@ -2533,11 +2551,11 @@
       </c>
     </row>
     <row r="136" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A136" s="23" t="s">
+      <c r="A136" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B136" s="23"/>
-      <c r="C136" s="23"/>
+      <c r="B136" s="36"/>
+      <c r="C136" s="36"/>
     </row>
     <row r="137" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
@@ -2585,11 +2603,11 @@
       <c r="C141" s="19"/>
     </row>
     <row r="142" spans="1:3" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A142" s="23" t="s">
+      <c r="A142" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="B142" s="23"/>
-      <c r="C142" s="23"/>
+      <c r="B142" s="36"/>
+      <c r="C142" s="36"/>
     </row>
     <row r="143" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
@@ -2612,30 +2630,30 @@
       </c>
     </row>
     <row r="147" spans="1:5" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C147" s="24" t="s">
+      <c r="C147" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D147" s="24"/>
+      <c r="D147" s="21"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148" s="21" t="s">
+      <c r="A148" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B148" s="21"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="21"/>
-      <c r="E148" s="21"/>
+      <c r="B148" s="37"/>
+      <c r="C148" s="37"/>
+      <c r="D148" s="37"/>
+      <c r="E148" s="37"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A149" s="22" t="s">
+      <c r="A149" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B149" s="22"/>
-      <c r="C149" s="22" t="s">
+      <c r="B149" s="38"/>
+      <c r="C149" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D149" s="22"/>
-      <c r="E149" s="22"/>
+      <c r="D149" s="38"/>
+      <c r="E149" s="38"/>
     </row>
     <row r="150" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
@@ -2672,24 +2690,24 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="21" t="s">
+      <c r="A153" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="B153" s="21"/>
-      <c r="C153" s="21"/>
-      <c r="D153" s="21"/>
-      <c r="E153" s="21"/>
+      <c r="B153" s="37"/>
+      <c r="C153" s="37"/>
+      <c r="D153" s="37"/>
+      <c r="E153" s="37"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="22" t="s">
+      <c r="A154" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B154" s="22"/>
-      <c r="C154" s="22" t="s">
+      <c r="B154" s="38"/>
+      <c r="C154" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="D154" s="22"/>
-      <c r="E154" s="22"/>
+      <c r="D154" s="38"/>
+      <c r="E154" s="38"/>
     </row>
     <row r="155" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
@@ -2726,13 +2744,13 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A158" s="25" t="s">
+      <c r="A158" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="B158" s="26"/>
-      <c r="C158" s="26"/>
-      <c r="D158" s="26"/>
-      <c r="E158" s="27"/>
+      <c r="B158" s="32"/>
+      <c r="C158" s="32"/>
+      <c r="D158" s="32"/>
+      <c r="E158" s="33"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="28" t="s">
@@ -2780,13 +2798,13 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A163" s="25" t="s">
+      <c r="A163" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B163" s="26"/>
-      <c r="C163" s="26"/>
-      <c r="D163" s="26"/>
-      <c r="E163" s="27"/>
+      <c r="B163" s="32"/>
+      <c r="C163" s="32"/>
+      <c r="D163" s="32"/>
+      <c r="E163" s="33"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="28" t="s">
@@ -2834,13 +2852,13 @@
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="25" t="s">
+      <c r="A168" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="B168" s="26"/>
-      <c r="C168" s="26"/>
-      <c r="D168" s="26"/>
-      <c r="E168" s="27"/>
+      <c r="B168" s="32"/>
+      <c r="C168" s="32"/>
+      <c r="D168" s="32"/>
+      <c r="E168" s="33"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="28" t="s">
@@ -2878,13 +2896,13 @@
       <c r="E171" s="1"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="25" t="s">
+      <c r="A173" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="B173" s="26"/>
-      <c r="C173" s="26"/>
-      <c r="D173" s="26"/>
-      <c r="E173" s="27"/>
+      <c r="B173" s="32"/>
+      <c r="C173" s="32"/>
+      <c r="D173" s="32"/>
+      <c r="E173" s="33"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="28" t="s">
@@ -2922,13 +2940,13 @@
       <c r="E176" s="1"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="25" t="s">
+      <c r="A178" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="B178" s="26"/>
-      <c r="C178" s="26"/>
-      <c r="D178" s="26"/>
-      <c r="E178" s="27"/>
+      <c r="B178" s="32"/>
+      <c r="C178" s="32"/>
+      <c r="D178" s="32"/>
+      <c r="E178" s="33"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="28" t="s">
@@ -2966,13 +2984,13 @@
       <c r="E181" s="1"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A183" s="25" t="s">
+      <c r="A183" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B183" s="26"/>
-      <c r="C183" s="26"/>
-      <c r="D183" s="26"/>
-      <c r="E183" s="27"/>
+      <c r="B183" s="32"/>
+      <c r="C183" s="32"/>
+      <c r="D183" s="32"/>
+      <c r="E183" s="33"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="28" t="s">
@@ -3010,10 +3028,10 @@
       <c r="E186" s="1"/>
     </row>
     <row r="188" spans="1:5" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C188" s="24" t="s">
+      <c r="C188" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D188" s="24"/>
+      <c r="D188" s="21"/>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B229" s="18" t="s">
@@ -3021,10 +3039,10 @@
       </c>
     </row>
     <row r="231" spans="2:4" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C231" s="24" t="s">
+      <c r="C231" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D231" s="24"/>
+      <c r="D231" s="21"/>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B233" s="18" t="s">
@@ -3032,16 +3050,16 @@
       </c>
     </row>
     <row r="235" spans="2:4" s="5" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C235" s="24" t="s">
+      <c r="C235" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D235" s="24"/>
+      <c r="D235" s="21"/>
     </row>
     <row r="271" spans="3:4" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C271" s="20" t="s">
+      <c r="C271" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="D271" s="20"/>
+      <c r="D271" s="44"/>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
@@ -3065,12 +3083,50 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C271:D271"/>
+    <mergeCell ref="A153:E153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="C154:E154"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="C235:D235"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="C179:E179"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C231:D231"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="A123:C123"/>
+    <mergeCell ref="A132:C132"/>
+    <mergeCell ref="A142:C142"/>
+    <mergeCell ref="A148:E148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="C149:E149"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="A43:G43"/>
@@ -3087,50 +3143,12 @@
     <mergeCell ref="A159:B159"/>
     <mergeCell ref="C159:E159"/>
     <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C231:D231"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="A123:C123"/>
-    <mergeCell ref="A132:C132"/>
-    <mergeCell ref="A142:C142"/>
-    <mergeCell ref="A148:E148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="C149:E149"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C271:D271"/>
-    <mergeCell ref="A153:E153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="C154:E154"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="C235:D235"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A179:B179"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Perbaiki sedikit tipo dari product backlognya
</commit_message>
<xml_diff>
--- a/Meme Agile.xlsx
+++ b/Meme Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\github\kelompok_meme_laporan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11158B5E-12A5-46C9-A10C-B8DA74C69CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130932A1-7155-49AB-A65B-8319141208D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BD1CD595-25D7-451D-99CB-E4C06CA26580}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="176">
   <si>
     <t>Product Backlog &amp; User Story</t>
   </si>
@@ -553,9 +553,6 @@
   </si>
   <si>
     <t>ada daya tarik yang kuat</t>
-  </si>
-  <si>
-    <t>Strong</t>
   </si>
 </sst>
 </file>
@@ -1506,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C4E763-3BF0-4DCE-A690-0A0674D041AB}">
   <dimension ref="A1:G279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I237" sqref="I237"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1949,7 +1946,7 @@
         <v>175</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>176</v>
+        <v>24</v>
       </c>
       <c r="G55" s="16">
         <v>5</v>

</xml_diff>

<commit_message>
koreksi penulisan Sprint Backlog
</commit_message>
<xml_diff>
--- a/Meme Agile.xlsx
+++ b/Meme Agile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13843d8ee8f93238/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{15DB3B59-8C40-47F8-B0B2-3A9F885E5C40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAD49B3D-F185-4200-A13E-F5E99E53CCFF}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{15DB3B59-8C40-47F8-B0B2-3A9F885E5C40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD07541C-8010-4BCD-A50F-292D21C04014}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{BD1CD595-25D7-451D-99CB-E4C06CA26580}"/>
   </bookViews>
@@ -564,7 +564,7 @@
     <t>Sebagai [Customer] memudahkan memberitahukan titik pengantaran</t>
   </si>
   <si>
-    <t>ada nya rating rekomdasi pembelian, sehingga membantu customer memilih produk yg banyak di pesan</t>
+    <t>Sebagai [CUSTOMER] ada nya rating rekomdasi pembelian, sehingga membantu customer memilih produk yg banyak di pesan</t>
   </si>
 </sst>
 </file>
@@ -831,8 +831,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -840,51 +888,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -894,16 +903,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1528,7 +1528,7 @@
   <dimension ref="A1:G281"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:B90"/>
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,23 +1543,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:5" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="3:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="4" spans="3:5" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="6" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
@@ -1590,18 +1590,18 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D22" s="9" t="s">
@@ -1690,15 +1690,15 @@
       <c r="A42" s="11"/>
     </row>
     <row r="43" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="48"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -2000,34 +2000,34 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="28"/>
+      <c r="B62" s="25"/>
     </row>
     <row r="63" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B63" s="28"/>
+      <c r="B63" s="25"/>
     </row>
     <row r="64" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="44" t="s">
+      <c r="A64" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B64" s="44"/>
+      <c r="B64" s="47"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="s">
+      <c r="A65" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="39"/>
+      <c r="B65" s="28"/>
     </row>
     <row r="66" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B66" s="28"/>
+      <c r="B66" s="25"/>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
@@ -2086,34 +2086,34 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B75" s="28"/>
+      <c r="B75" s="25"/>
     </row>
     <row r="76" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="28"/>
+      <c r="B76" s="25"/>
     </row>
     <row r="77" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="37" t="s">
+      <c r="A77" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B77" s="37"/>
+      <c r="B77" s="26"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B78" s="39"/>
+      <c r="B78" s="28"/>
     </row>
     <row r="79" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="40" t="s">
+      <c r="A79" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B79" s="40"/>
+      <c r="B79" s="24"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
@@ -2132,34 +2132,34 @@
       </c>
     </row>
     <row r="83" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="28"/>
+      <c r="B83" s="25"/>
     </row>
     <row r="84" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B84" s="28"/>
+      <c r="B84" s="25"/>
     </row>
     <row r="85" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="37" t="s">
+      <c r="A85" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="37"/>
+      <c r="B85" s="26"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="38" t="s">
+      <c r="A86" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B86" s="39"/>
+      <c r="B86" s="28"/>
     </row>
     <row r="87" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="40" t="s">
+      <c r="A87" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B87" s="40"/>
+      <c r="B87" s="24"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -2177,7 +2177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="21">
         <v>560</v>
       </c>
@@ -2186,32 +2186,32 @@
       </c>
     </row>
     <row r="92" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B92" s="28"/>
+      <c r="B92" s="25"/>
     </row>
     <row r="93" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="28" t="s">
+      <c r="A93" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B93" s="28"/>
+      <c r="B93" s="25"/>
     </row>
     <row r="94" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A94" s="37" t="s">
+      <c r="A94" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B94" s="37"/>
+      <c r="B94" s="26"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="38"/>
-      <c r="B95" s="39"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="28"/>
     </row>
     <row r="96" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A96" s="40" t="s">
+      <c r="A96" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B96" s="40"/>
+      <c r="B96" s="24"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
@@ -2238,32 +2238,32 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B101" s="28"/>
+      <c r="B101" s="25"/>
     </row>
     <row r="102" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="B102" s="28"/>
+      <c r="B102" s="25"/>
     </row>
     <row r="103" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="37" t="s">
+      <c r="A103" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B103" s="37"/>
+      <c r="B103" s="26"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="38"/>
-      <c r="B104" s="39"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="28"/>
     </row>
     <row r="105" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A105" s="40" t="s">
+      <c r="A105" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B105" s="40"/>
+      <c r="B105" s="24"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
@@ -2290,10 +2290,10 @@
       </c>
     </row>
     <row r="110" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C110" s="28" t="s">
+      <c r="C110" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D110" s="28"/>
+      <c r="D110" s="25"/>
     </row>
     <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
@@ -2536,17 +2536,17 @@
       </c>
     </row>
     <row r="124" spans="1:6" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C124" s="28" t="s">
+      <c r="C124" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D124" s="28"/>
+      <c r="D124" s="25"/>
     </row>
     <row r="125" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A125" s="45" t="s">
+      <c r="A125" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="B125" s="45"/>
-      <c r="C125" s="45"/>
+      <c r="B125" s="39"/>
+      <c r="C125" s="39"/>
     </row>
     <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
@@ -2608,11 +2608,11 @@
       <c r="C132" s="1"/>
     </row>
     <row r="134" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="27" t="s">
+      <c r="A134" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B134" s="27"/>
-      <c r="C134" s="27"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="40"/>
     </row>
     <row r="135" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
@@ -2637,11 +2637,11 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="27" t="s">
+      <c r="A138" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B138" s="27"/>
-      <c r="C138" s="27"/>
+      <c r="B138" s="40"/>
+      <c r="C138" s="40"/>
     </row>
     <row r="139" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
@@ -2689,11 +2689,11 @@
       <c r="C143" s="19"/>
     </row>
     <row r="144" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="27" t="s">
+      <c r="A144" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B144" s="27"/>
-      <c r="C144" s="27"/>
+      <c r="B144" s="40"/>
+      <c r="C144" s="40"/>
     </row>
     <row r="145" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
@@ -2716,30 +2716,30 @@
       </c>
     </row>
     <row r="149" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C149" s="28" t="s">
+      <c r="C149" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D149" s="28"/>
+      <c r="D149" s="25"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="25" t="s">
+      <c r="A150" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B150" s="25"/>
-      <c r="C150" s="25"/>
-      <c r="D150" s="25"/>
-      <c r="E150" s="25"/>
+      <c r="B150" s="41"/>
+      <c r="C150" s="41"/>
+      <c r="D150" s="41"/>
+      <c r="E150" s="41"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="26" t="s">
+      <c r="A151" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B151" s="26"/>
-      <c r="C151" s="26" t="s">
+      <c r="B151" s="42"/>
+      <c r="C151" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D151" s="26"/>
-      <c r="E151" s="26"/>
+      <c r="D151" s="42"/>
+      <c r="E151" s="42"/>
     </row>
     <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
@@ -2776,24 +2776,24 @@
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="25" t="s">
+      <c r="A155" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="B155" s="25"/>
-      <c r="C155" s="25"/>
-      <c r="D155" s="25"/>
-      <c r="E155" s="25"/>
+      <c r="B155" s="41"/>
+      <c r="C155" s="41"/>
+      <c r="D155" s="41"/>
+      <c r="E155" s="41"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="26" t="s">
+      <c r="A156" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B156" s="26"/>
-      <c r="C156" s="26" t="s">
+      <c r="B156" s="42"/>
+      <c r="C156" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D156" s="26"/>
-      <c r="E156" s="26"/>
+      <c r="D156" s="42"/>
+      <c r="E156" s="42"/>
     </row>
     <row r="157" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
@@ -2830,13 +2830,13 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="29" t="s">
+      <c r="A160" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B160" s="30"/>
-      <c r="C160" s="30"/>
-      <c r="D160" s="30"/>
-      <c r="E160" s="31"/>
+      <c r="B160" s="36"/>
+      <c r="C160" s="36"/>
+      <c r="D160" s="36"/>
+      <c r="E160" s="37"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="32" t="s">
@@ -2884,13 +2884,13 @@
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="29" t="s">
+      <c r="A165" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="B165" s="30"/>
-      <c r="C165" s="30"/>
-      <c r="D165" s="30"/>
-      <c r="E165" s="31"/>
+      <c r="B165" s="36"/>
+      <c r="C165" s="36"/>
+      <c r="D165" s="36"/>
+      <c r="E165" s="37"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="32" t="s">
@@ -2938,13 +2938,13 @@
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="29" t="s">
+      <c r="A170" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="B170" s="30"/>
-      <c r="C170" s="30"/>
-      <c r="D170" s="30"/>
-      <c r="E170" s="31"/>
+      <c r="B170" s="36"/>
+      <c r="C170" s="36"/>
+      <c r="D170" s="36"/>
+      <c r="E170" s="37"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="32" t="s">
@@ -2982,13 +2982,13 @@
       <c r="E173" s="1"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="29" t="s">
+      <c r="A175" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="B175" s="30"/>
-      <c r="C175" s="30"/>
-      <c r="D175" s="30"/>
-      <c r="E175" s="31"/>
+      <c r="B175" s="36"/>
+      <c r="C175" s="36"/>
+      <c r="D175" s="36"/>
+      <c r="E175" s="37"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="32" t="s">
@@ -3026,13 +3026,13 @@
       <c r="E178" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="29" t="s">
+      <c r="A180" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="B180" s="30"/>
-      <c r="C180" s="30"/>
-      <c r="D180" s="30"/>
-      <c r="E180" s="31"/>
+      <c r="B180" s="36"/>
+      <c r="C180" s="36"/>
+      <c r="D180" s="36"/>
+      <c r="E180" s="37"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="32" t="s">
@@ -3070,13 +3070,13 @@
       <c r="E183" s="1"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="29" t="s">
+      <c r="A185" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="B185" s="30"/>
-      <c r="C185" s="30"/>
-      <c r="D185" s="30"/>
-      <c r="E185" s="31"/>
+      <c r="B185" s="36"/>
+      <c r="C185" s="36"/>
+      <c r="D185" s="36"/>
+      <c r="E185" s="37"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="32" t="s">
@@ -3114,10 +3114,10 @@
       <c r="E188" s="1"/>
     </row>
     <row r="190" spans="1:5" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C190" s="28" t="s">
+      <c r="C190" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D190" s="28"/>
+      <c r="D190" s="25"/>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="18" t="s">
@@ -3126,10 +3126,10 @@
       <c r="C231" s="18"/>
     </row>
     <row r="233" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C233" s="28" t="s">
+      <c r="C233" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D233" s="28"/>
+      <c r="D233" s="25"/>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B235" s="18" t="s">
@@ -3138,16 +3138,16 @@
       <c r="C235" s="18"/>
     </row>
     <row r="237" spans="2:4" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C237" s="28" t="s">
+      <c r="C237" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D237" s="28"/>
+      <c r="D237" s="25"/>
     </row>
     <row r="273" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C273" s="24" t="s">
+      <c r="C273" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="D273" s="24"/>
+      <c r="D273" s="48"/>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
@@ -3171,12 +3171,50 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C273:D273"/>
+    <mergeCell ref="A155:E155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="A138:C138"/>
+    <mergeCell ref="C237:D237"/>
+    <mergeCell ref="A180:E180"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="A175:E175"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C233:D233"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="A125:C125"/>
+    <mergeCell ref="A134:C134"/>
+    <mergeCell ref="A144:C144"/>
+    <mergeCell ref="A150:E150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="C151:E151"/>
+    <mergeCell ref="A185:E185"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="A43:G43"/>
@@ -3193,50 +3231,12 @@
     <mergeCell ref="A161:B161"/>
     <mergeCell ref="C161:E161"/>
     <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C233:D233"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="A125:C125"/>
-    <mergeCell ref="A134:C134"/>
-    <mergeCell ref="A144:C144"/>
-    <mergeCell ref="A150:E150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="C151:E151"/>
-    <mergeCell ref="A185:E185"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C273:D273"/>
-    <mergeCell ref="A155:E155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="C156:E156"/>
-    <mergeCell ref="A138:C138"/>
-    <mergeCell ref="C237:D237"/>
-    <mergeCell ref="A180:E180"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="A175:E175"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>